<commit_message>
Run linear standard analysis
</commit_message>
<xml_diff>
--- a/hyper/Configuration.xlsx
+++ b/hyper/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\hyper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0A9541-BA5E-4A82-A671-1BB94FCFD3CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27F091A-C9BA-4C97-9BF9-486E43079604}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="112">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t>car</t>
+  </si>
+  <si>
+    <t>Fails</t>
+  </si>
+  <si>
+    <t>Timeout</t>
   </si>
 </sst>
 </file>
@@ -1211,10 +1217,10 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,1037 +1308,1037 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>80</v>
+      <c r="A8" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>100</v>
       </c>
       <c r="C8">
-        <v>34539</v>
+        <v>3560</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
         <v>100</v>
       </c>
       <c r="C9">
-        <v>3560</v>
+        <v>14971</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
         <v>100</v>
       </c>
       <c r="C10">
-        <v>14971</v>
+        <v>146802</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>100</v>
       </c>
       <c r="C11">
-        <v>146802</v>
+        <v>9976</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
         <v>100</v>
       </c>
       <c r="C12">
-        <v>9976</v>
+        <v>125920</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>100</v>
       </c>
       <c r="C13">
-        <v>125920</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
         <v>100</v>
       </c>
       <c r="C14">
-        <v>22</v>
+        <v>14965</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
         <v>100</v>
       </c>
       <c r="C15">
-        <v>14969</v>
+        <v>146195</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
         <v>100</v>
       </c>
       <c r="C16">
-        <v>14965</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
         <v>100</v>
       </c>
       <c r="C17">
-        <v>146195</v>
+        <v>3889</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>100</v>
       </c>
       <c r="C18">
-        <v>3896</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
         <v>100</v>
       </c>
       <c r="C19">
-        <v>3889</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
         <v>100</v>
       </c>
       <c r="C20">
-        <v>21</v>
+        <v>146606</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>100</v>
       </c>
       <c r="C21">
-        <v>3573</v>
+        <v>14970</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
         <v>100</v>
       </c>
       <c r="C22">
-        <v>3946</v>
+        <v>14966</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="2">
-        <v>3948</v>
+      <c r="C23">
+        <v>9977</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
         <v>100</v>
       </c>
       <c r="C24">
-        <v>146606</v>
+        <v>146607</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
         <v>100</v>
       </c>
       <c r="C25">
-        <v>14970</v>
+        <v>9986</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
         <v>100</v>
       </c>
       <c r="C26">
-        <v>14966</v>
+        <v>9964</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
         <v>100</v>
       </c>
       <c r="C27">
-        <v>9977</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
         <v>100</v>
       </c>
       <c r="C28">
-        <v>146607</v>
+        <v>3891</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>100</v>
       </c>
       <c r="C29">
-        <v>9986</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
         <v>100</v>
       </c>
       <c r="C30">
-        <v>9964</v>
+        <v>9981</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>100</v>
       </c>
       <c r="C31">
-        <v>20</v>
+        <v>9950</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
         <v>100</v>
       </c>
       <c r="C32">
-        <v>3891</v>
+        <v>14968</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>100</v>
       </c>
       <c r="C33">
-        <v>3481</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>58</v>
+      <c r="A34" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>100</v>
       </c>
       <c r="C34">
-        <v>9981</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
         <v>100</v>
       </c>
       <c r="C35">
-        <v>9950</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
         <v>100</v>
       </c>
       <c r="C36">
-        <v>14968</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
         <v>100</v>
       </c>
       <c r="C37">
-        <v>2125</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>32</v>
+      <c r="A38" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B38" t="s">
         <v>100</v>
       </c>
       <c r="C38">
-        <v>3493</v>
+        <v>9980</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
         <v>100</v>
       </c>
       <c r="C39">
-        <v>53</v>
+        <v>146820</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
         <v>100</v>
       </c>
       <c r="C40">
-        <v>31</v>
+        <v>146800</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
         <v>100</v>
       </c>
       <c r="C41">
-        <v>29</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
         <v>100</v>
       </c>
       <c r="C42">
-        <v>9980</v>
+        <v>9954</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
         <v>100</v>
       </c>
       <c r="C43">
-        <v>146820</v>
+        <v>9955</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
         <v>100</v>
       </c>
       <c r="C44">
-        <v>146800</v>
+        <v>9956</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
         <v>100</v>
       </c>
       <c r="C45">
-        <v>2075</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
         <v>100</v>
       </c>
       <c r="C46">
-        <v>9954</v>
+        <v>14964</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>100</v>
       </c>
       <c r="C47">
-        <v>9955</v>
+        <v>9985</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
         <v>100</v>
       </c>
       <c r="C48">
-        <v>9956</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
         <v>100</v>
       </c>
       <c r="C49">
-        <v>219</v>
+        <v>145804</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
         <v>100</v>
       </c>
       <c r="C50">
-        <v>14964</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
         <v>100</v>
       </c>
       <c r="C51">
-        <v>9985</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
         <v>100</v>
       </c>
       <c r="C52">
-        <v>3954</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
         <v>100</v>
       </c>
       <c r="C53">
-        <v>145804</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
         <v>100</v>
       </c>
       <c r="C54">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
         <v>100</v>
       </c>
       <c r="C55">
-        <v>3021</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
         <v>100</v>
       </c>
       <c r="C56">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
         <v>100</v>
       </c>
       <c r="C57">
-        <v>1779</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B58" t="s">
         <v>100</v>
       </c>
       <c r="C58">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
         <v>100</v>
       </c>
       <c r="C59">
-        <v>1788</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B60" t="s">
         <v>100</v>
       </c>
       <c r="C60">
-        <v>28</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
         <v>100</v>
       </c>
       <c r="C61">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
         <v>100</v>
       </c>
       <c r="C62">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
         <v>100</v>
       </c>
       <c r="C63">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B64" t="s">
         <v>100</v>
       </c>
       <c r="C64">
-        <v>1778</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
         <v>100</v>
       </c>
       <c r="C65">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
         <v>100</v>
       </c>
       <c r="C66">
-        <v>36</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
         <v>100</v>
       </c>
       <c r="C67">
-        <v>43</v>
+        <v>3485</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
         <v>100</v>
       </c>
-      <c r="C68">
-        <v>45</v>
+      <c r="C68" s="2">
+        <v>3492</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B69" t="s">
         <v>100</v>
       </c>
       <c r="C69">
-        <v>58</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B70" t="s">
         <v>100</v>
       </c>
       <c r="C70">
-        <v>2074</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B71" t="s">
         <v>100</v>
       </c>
       <c r="C71">
-        <v>3485</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B72" t="s">
         <v>100</v>
       </c>
-      <c r="C72" s="2">
-        <v>3492</v>
+      <c r="C72">
+        <v>3543</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B73" t="s">
         <v>100</v>
       </c>
       <c r="C73">
-        <v>3494</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B74" t="s">
         <v>100</v>
       </c>
       <c r="C74">
-        <v>4544</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B75" t="s">
         <v>100</v>
       </c>
       <c r="C75">
-        <v>3512</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B76" t="s">
         <v>100</v>
       </c>
       <c r="C76">
-        <v>3543</v>
+        <v>3903</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B77" t="s">
         <v>100</v>
       </c>
       <c r="C77">
-        <v>3549</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B78" t="s">
         <v>100</v>
       </c>
       <c r="C78">
-        <v>3899</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B79" t="s">
         <v>100</v>
       </c>
       <c r="C79">
-        <v>3902</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B80" t="s">
         <v>100</v>
       </c>
       <c r="C80">
-        <v>3903</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B81" t="s">
         <v>100</v>
       </c>
-      <c r="C81">
-        <v>3904</v>
+      <c r="C81" s="2">
+        <v>10093</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B82" t="s">
         <v>100</v>
       </c>
       <c r="C82">
-        <v>3913</v>
+        <v>10101</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B83" t="s">
         <v>100</v>
       </c>
       <c r="C83">
-        <v>3917</v>
+        <v>9979</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B84" t="s">
         <v>100</v>
       </c>
       <c r="C84">
-        <v>3918</v>
+        <v>9983</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B85" t="s">
         <v>100</v>
       </c>
-      <c r="C85" s="2">
-        <v>10093</v>
+      <c r="C85">
+        <v>9970</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B86" t="s">
         <v>100</v>
       </c>
       <c r="C86">
-        <v>10101</v>
+        <v>9971</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B87" t="s">
         <v>100</v>
       </c>
       <c r="C87">
-        <v>9979</v>
+        <v>9978</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B88" t="s">
         <v>100</v>
       </c>
       <c r="C88">
-        <v>9983</v>
+        <v>9952</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B89" t="s">
         <v>100</v>
       </c>
       <c r="C89">
-        <v>9970</v>
+        <v>9957</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B90" t="s">
         <v>100</v>
       </c>
       <c r="C90">
-        <v>9971</v>
+        <v>9960</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B91" t="s">
         <v>100</v>
       </c>
       <c r="C91">
-        <v>9978</v>
+        <v>9967</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B92" t="s">
         <v>100</v>
       </c>
       <c r="C92">
-        <v>9952</v>
+        <v>9946</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
         <v>100</v>
       </c>
       <c r="C93">
-        <v>9957</v>
+        <v>7592</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B94" t="s">
         <v>100</v>
       </c>
       <c r="C94">
-        <v>9960</v>
+        <v>14967</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B95" t="s">
         <v>100</v>
       </c>
       <c r="C95">
-        <v>9967</v>
+        <v>125921</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B96" t="s">
         <v>100</v>
       </c>
       <c r="C96">
-        <v>9946</v>
+        <v>125922</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B97" t="s">
         <v>100</v>
       </c>
       <c r="C97">
-        <v>7592</v>
+        <v>34537</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>84</v>
+      <c r="A98" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C98">
-        <v>14967</v>
+        <v>34539</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
         <v>100</v>
       </c>
       <c r="C99">
-        <v>125921</v>
+        <v>14969</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C100">
-        <v>125922</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B101" t="s">
-        <v>100</v>
-      </c>
-      <c r="C101">
-        <v>34537</v>
+        <v>110</v>
+      </c>
+      <c r="C101" s="2">
+        <v>3948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>